<commit_message>
fixed custom system prompt + voice effects + robocop added
</commit_message>
<xml_diff>
--- a/lib/l10n/strings.xlsx
+++ b/lib/l10n/strings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -183,6 +183,15 @@
   <si>
     <t xml:space="preserve">For more voices : ‘Google Text-to-Speech’ on the Play Store</t>
   </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Votre nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your name</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +348,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,8 +619,8 @@
   </sheetPr>
   <dimension ref="A1:CB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2292,9 +2301,15 @@
       <c r="CB19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>

</xml_diff>

<commit_message>
function calling (get weather and get last news) + christmas assets
</commit_message>
<xml_diff>
--- a/lib/l10n/strings.xlsx
+++ b/lib/l10n/strings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t xml:space="preserve">User’s name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resultsFunctionCalling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résultats de functions calling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function calling results</t>
   </si>
 </sst>
 </file>
@@ -611,7 +620,7 @@
   <dimension ref="A1:CB1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2292,9 +2301,15 @@
       <c r="CB19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>

</xml_diff>

<commit_message>
persona prompts update + readme
</commit_message>
<xml_diff>
--- a/lib/l10n/strings.xlsx
+++ b/lib/l10n/strings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t xml:space="preserve">Function calling results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personaAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personnalité de l’assistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant’s persona</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
   <dimension ref="A1:CB1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2389,9 +2398,15 @@
       <c r="CB20" s="7"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>

</xml_diff>